<commit_message>
Revert "Merge branch 'master' of https://github.com/hgkj-rj-02/hgkj_02"
This reverts commit e6abb88142ed26bee36516df65e77447b512e721, reversing
changes made to 1f36371e01d8e990d8e515621b2567bdff58006f.
</commit_message>
<xml_diff>
--- a/樊佩茹/项目进度控制表-樊佩茹 .xlsx
+++ b/樊佩茹/项目进度控制表-樊佩茹 .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SDX\Desktop\hgkj_02\樊佩茹\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFDAEBF-9431-4D87-9E59-4A25FA5F8A23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="4"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="樊佩茹" sheetId="1" r:id="rId1"/>
@@ -214,7 +220,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,73 +658,73 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -776,7 +782,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -809,9 +815,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,6 +867,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1019,33 +1059,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.625" customWidth="1"/>
-    <col min="2" max="2" width="29.75" customWidth="1"/>
-    <col min="3" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="84.625" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="29.7265625" customWidth="1"/>
+    <col min="3" max="6" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="84.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1068,25 +1108,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="44" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="69" t="s">
+    <row r="3" spans="1:7" s="44" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
-    </row>
-    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="67">
         <v>43638</v>
       </c>
       <c r="D4" s="11"/>
@@ -1100,14 +1140,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12">
         <v>43640</v>
@@ -1117,8 +1157,8 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="80" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -1138,12 +1178,12 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="81"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="67">
         <v>43640</v>
       </c>
       <c r="D7" s="12"/>
@@ -1157,12 +1197,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="82"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="82"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="12">
         <v>43641</v>
       </c>
@@ -1174,14 +1214,14 @@
       </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="64" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="67">
         <v>43641</v>
       </c>
       <c r="D9" s="12"/>
@@ -1193,12 +1233,12 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="66"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="83"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12">
         <v>43642</v>
@@ -1210,12 +1250,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="65"/>
       <c r="B11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12">
         <v>43642</v>
@@ -1225,14 +1265,14 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="64" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="81">
+      <c r="C12" s="67">
         <v>43642</v>
       </c>
       <c r="D12" s="12"/>
@@ -1240,58 +1280,58 @@
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="66"/>
       <c r="B13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="66"/>
       <c r="B14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="65"/>
       <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="25"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="72" t="s">
+    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="78" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="64" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="81">
+      <c r="C17" s="67">
         <v>43643</v>
       </c>
       <c r="D17" s="12"/>
@@ -1299,25 +1339,25 @@
       <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="65"/>
       <c r="B18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="12"/>
@@ -1325,23 +1365,23 @@
       <c r="F19" s="25"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="66"/>
       <c r="B20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="25"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="66"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="67">
         <v>43646</v>
       </c>
       <c r="D21" s="12"/>
@@ -1349,25 +1389,25 @@
       <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="65"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="s">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="64" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="70" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="12"/>
@@ -1375,36 +1415,36 @@
       <c r="F23" s="25"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="79"/>
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="66"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="65"/>
       <c r="B25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="78" t="s">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="64" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="67">
         <v>43650</v>
       </c>
       <c r="D26" s="12"/>
@@ -1412,34 +1452,34 @@
       <c r="F26" s="25"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="79"/>
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="66"/>
       <c r="B27" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="83"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="25"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="79"/>
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="66"/>
       <c r="B28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="66"/>
       <c r="B29" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="81">
+      <c r="C29" s="67">
         <v>43651</v>
       </c>
       <c r="D29" s="12"/>
@@ -1447,23 +1487,23 @@
       <c r="F29" s="25"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="65"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="25"/>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A31" s="11"/>
       <c r="B31" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -1471,6 +1511,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A15"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A25"/>
@@ -1485,12 +1531,6 @@
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1499,36 +1539,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.875" customWidth="1"/>
-    <col min="2" max="2" width="32.875" customWidth="1"/>
-    <col min="3" max="3" width="15.125" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="81.125" customWidth="1"/>
+    <col min="1" max="1" width="18.90625" customWidth="1"/>
+    <col min="2" max="2" width="32.90625" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="81.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+    </row>
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1551,25 +1591,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="69" t="s">
+    <row r="3" spans="1:7" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="67">
         <v>43638</v>
       </c>
       <c r="D4" s="11"/>
@@ -1583,14 +1623,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12">
         <v>43640</v>
@@ -1600,8 +1640,8 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="80" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -1619,12 +1659,12 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="81"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="67">
         <v>43640</v>
       </c>
       <c r="D7" s="12"/>
@@ -1638,25 +1678,25 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="82"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="82"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="25"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="64" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="67">
         <v>43641</v>
       </c>
       <c r="D9" s="12"/>
@@ -1664,12 +1704,12 @@
       <c r="F9" s="25"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="66"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="83"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12">
         <v>43642</v>
@@ -1681,25 +1721,25 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="65"/>
       <c r="B11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="64" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="81">
+      <c r="C12" s="67">
         <v>43642</v>
       </c>
       <c r="D12" s="12"/>
@@ -1707,12 +1747,12 @@
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="66"/>
       <c r="B13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12">
         <v>43642</v>
@@ -1724,12 +1764,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="66"/>
       <c r="B14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12">
         <v>43642</v>
@@ -1741,36 +1781,36 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="65"/>
       <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="25"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="72" t="s">
+    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="78" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="64" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="81">
+      <c r="C17" s="67">
         <v>43643</v>
       </c>
       <c r="D17" s="12"/>
@@ -1778,25 +1818,25 @@
       <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="65"/>
       <c r="B18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="12"/>
@@ -1804,23 +1844,23 @@
       <c r="F19" s="25"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="66"/>
       <c r="B20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="25"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="66"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="67">
         <v>43646</v>
       </c>
       <c r="D21" s="12"/>
@@ -1828,25 +1868,25 @@
       <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="65"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="s">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="64" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="70" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="12"/>
@@ -1854,36 +1894,36 @@
       <c r="F23" s="25"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="79"/>
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="66"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="65"/>
       <c r="B25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="78" t="s">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="64" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="67">
         <v>43650</v>
       </c>
       <c r="D26" s="12"/>
@@ -1891,34 +1931,34 @@
       <c r="F26" s="25"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="79"/>
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="66"/>
       <c r="B27" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="83"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="25"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="79"/>
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="66"/>
       <c r="B28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="66"/>
       <c r="B29" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="81">
+      <c r="C29" s="67">
         <v>43651</v>
       </c>
       <c r="D29" s="12"/>
@@ -1926,23 +1966,23 @@
       <c r="F29" s="25"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="65"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="25"/>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A31" s="11"/>
       <c r="B31" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -1950,6 +1990,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A15"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A25"/>
@@ -1964,12 +2010,6 @@
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1978,25 +2018,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="31.625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="31.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="87.625" customWidth="1"/>
+    <col min="7" max="7" width="87.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2007,7 +2047,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2030,7 +2070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -2041,7 +2081,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -2062,7 +2102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
@@ -2079,7 +2119,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
         <v>14</v>
       </c>
@@ -2098,9 +2138,9 @@
       <c r="F6" s="13">
         <v>1</v>
       </c>
-      <c r="G6" s="65"/>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G6" s="84"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" s="19"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
@@ -2117,11 +2157,11 @@
       <c r="F7" s="13">
         <v>0.8</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="84" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A8" s="20"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
@@ -2136,7 +2176,7 @@
       </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A9" s="21" t="s">
         <v>18</v>
       </c>
@@ -2155,7 +2195,7 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A10" s="22"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
@@ -2168,11 +2208,11 @@
       <c r="F10" s="13">
         <v>0.8</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="84" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A11" s="24"/>
       <c r="B11" s="16" t="s">
         <v>21</v>
@@ -2183,7 +2223,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A12" s="21" t="s">
         <v>22</v>
       </c>
@@ -2202,11 +2242,11 @@
       <c r="F12" s="13">
         <v>0.8</v>
       </c>
-      <c r="G12" s="65" t="s">
+      <c r="G12" s="84" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A13" s="22"/>
       <c r="B13" s="16" t="s">
         <v>24</v>
@@ -2217,7 +2257,7 @@
       <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A14" s="22"/>
       <c r="B14" s="16" t="s">
         <v>25</v>
@@ -2228,7 +2268,7 @@
       <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A15" s="24"/>
       <c r="B15" s="16" t="s">
         <v>26</v>
@@ -2239,7 +2279,7 @@
       <c r="F15" s="25"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>27</v>
       </c>
@@ -2250,7 +2290,7 @@
       <c r="F16" s="27"/>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A17" s="21" t="s">
         <v>28</v>
       </c>
@@ -2265,7 +2305,7 @@
       <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A18" s="24"/>
       <c r="B18" s="16" t="s">
         <v>30</v>
@@ -2276,7 +2316,7 @@
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A19" s="21" t="s">
         <v>31</v>
       </c>
@@ -2291,7 +2331,7 @@
       <c r="F19" s="25"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A20" s="22"/>
       <c r="B20" s="16" t="s">
         <v>34</v>
@@ -2302,7 +2342,7 @@
       <c r="F20" s="25"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A21" s="22"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
@@ -2315,7 +2355,7 @@
       <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A22" s="24"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -2326,7 +2366,7 @@
       <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="33" x14ac:dyDescent="0.45">
       <c r="A23" s="21" t="s">
         <v>37</v>
       </c>
@@ -2341,7 +2381,7 @@
       <c r="F23" s="25"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A24" s="22"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -2352,7 +2392,7 @@
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A25" s="24"/>
       <c r="B25" s="16" t="s">
         <v>41</v>
@@ -2363,7 +2403,7 @@
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A26" s="21" t="s">
         <v>42</v>
       </c>
@@ -2378,7 +2418,7 @@
       <c r="F26" s="25"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A27" s="22"/>
       <c r="B27" s="16" t="s">
         <v>44</v>
@@ -2389,7 +2429,7 @@
       <c r="F27" s="25"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A28" s="22"/>
       <c r="B28" s="16" t="s">
         <v>45</v>
@@ -2400,7 +2440,7 @@
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A29" s="22"/>
       <c r="B29" s="16" t="s">
         <v>46</v>
@@ -2413,7 +2453,7 @@
       <c r="F29" s="25"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A30" s="24"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
@@ -2424,7 +2464,7 @@
       <c r="F30" s="25"/>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A31" s="11"/>
       <c r="B31" s="9" t="s">
         <v>48</v>
@@ -2443,37 +2483,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="32" customWidth="1"/>
-    <col min="2" max="2" width="18.625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="25.375" style="32" customWidth="1"/>
-    <col min="4" max="4" width="18.875" style="32" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="32" customWidth="1"/>
-    <col min="6" max="6" width="16.625" style="32" customWidth="1"/>
-    <col min="7" max="7" width="47.375" style="32" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" style="32" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="47.36328125" style="32" customWidth="1"/>
     <col min="8" max="16384" width="11" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2496,25 +2536,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="69" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="67">
         <v>43638</v>
       </c>
       <c r="D4" s="35"/>
@@ -2526,14 +2566,14 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="13">
@@ -2541,7 +2581,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>14</v>
       </c>
@@ -2558,12 +2598,12 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="67">
         <v>43640</v>
       </c>
       <c r="D7" s="12"/>
@@ -2573,12 +2613,12 @@
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A8" s="38"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="82"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13">
@@ -2586,14 +2626,14 @@
       </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A9" s="39" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="67">
         <v>43641</v>
       </c>
       <c r="D9" s="12"/>
@@ -2603,12 +2643,12 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A10" s="38"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="83"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13">
@@ -2616,12 +2656,12 @@
       </c>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A11" s="40"/>
       <c r="B11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13">
@@ -2629,14 +2669,14 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A12" s="39" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="81">
+      <c r="C12" s="67">
         <v>43642</v>
       </c>
       <c r="D12" s="12"/>
@@ -2644,58 +2684,58 @@
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A13" s="15"/>
       <c r="B13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A14" s="41"/>
       <c r="B14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A15" s="42"/>
       <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="25"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="72" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A17" s="39" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="81">
+      <c r="C17" s="67">
         <v>43643</v>
       </c>
       <c r="D17" s="12"/>
@@ -2703,25 +2743,25 @@
       <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A18" s="42"/>
       <c r="B18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A19" s="39" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="12"/>
@@ -2729,23 +2769,23 @@
       <c r="F19" s="25"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A20" s="42"/>
       <c r="B20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="25"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A21" s="42"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="67">
         <v>43646</v>
       </c>
       <c r="D21" s="12"/>
@@ -2753,25 +2793,25 @@
       <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A22" s="41"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A23" s="39" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="70" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="12"/>
@@ -2779,36 +2819,36 @@
       <c r="F23" s="25"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A24" s="40"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A25" s="40"/>
       <c r="B25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="27" x14ac:dyDescent="0.45">
       <c r="A26" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="67">
         <v>43650</v>
       </c>
       <c r="D26" s="12"/>
@@ -2816,34 +2856,34 @@
       <c r="F26" s="25"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A27" s="40"/>
       <c r="B27" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="83"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="25"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A28" s="42"/>
       <c r="B28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A29" s="42"/>
       <c r="B29" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="81">
+      <c r="C29" s="67">
         <v>43651</v>
       </c>
       <c r="D29" s="12"/>
@@ -2851,23 +2891,23 @@
       <c r="F29" s="25"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A30" s="15"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="25"/>
       <c r="G30" s="43"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A31" s="35"/>
       <c r="B31" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
       <c r="F31" s="35"/>
@@ -2875,12 +2915,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C26:C28"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A16:G16"/>
@@ -2888,6 +2922,12 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C26:C28"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -2895,36 +2935,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="31.625" customWidth="1"/>
-    <col min="3" max="3" width="14.75" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
-    <col min="5" max="5" width="15.625" customWidth="1"/>
-    <col min="6" max="6" width="14.875" customWidth="1"/>
-    <col min="7" max="7" width="90.75" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" customWidth="1"/>
+    <col min="7" max="7" width="90.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+    </row>
+    <row r="2" spans="1:7" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2947,25 +2987,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="69" t="s">
+    <row r="3" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="67">
         <v>43638</v>
       </c>
       <c r="D4" s="11"/>
@@ -2979,14 +3019,14 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12">
         <v>43640</v>
@@ -2996,8 +3036,8 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="80" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -3006,23 +3046,21 @@
       <c r="C6" s="12">
         <v>43639</v>
       </c>
-      <c r="D6" s="12">
-        <v>43643</v>
-      </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="12">
         <v>43640</v>
       </c>
       <c r="F6" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="81"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="67">
         <v>43640</v>
       </c>
       <c r="D7" s="12"/>
@@ -3030,36 +3068,35 @@
         <v>43641</v>
       </c>
       <c r="F7" s="13">
-        <v>0.9</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="82"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="12">
-        <v>43643</v>
-      </c>
+      <c r="C8" s="68"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="12">
         <v>43641</v>
       </c>
       <c r="F8" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="64" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="67">
         <v>43641</v>
       </c>
       <c r="D9" s="12"/>
@@ -3071,44 +3108,44 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="66"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="83"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12">
         <v>43641</v>
       </c>
       <c r="F10" s="13">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="65"/>
       <c r="B11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12">
         <v>43641</v>
       </c>
       <c r="F11" s="13">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="64" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="81">
+      <c r="C12" s="67">
         <v>43642</v>
       </c>
       <c r="D12" s="12"/>
@@ -3122,12 +3159,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="66"/>
       <c r="B13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12">
         <v>43642</v>
@@ -3137,12 +3174,12 @@
       </c>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="66"/>
       <c r="B14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12">
         <v>43642</v>
@@ -3152,12 +3189,12 @@
       </c>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="65"/>
       <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12">
         <v>43642</v>
@@ -3167,25 +3204,25 @@
       </c>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="72" t="s">
+    <row r="16" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="78" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="64" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="81">
+      <c r="C17" s="67">
         <v>43643</v>
       </c>
       <c r="D17" s="12"/>
@@ -3193,25 +3230,25 @@
       <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="65"/>
       <c r="B18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="12"/>
@@ -3219,23 +3256,23 @@
       <c r="F19" s="25"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="66"/>
       <c r="B20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="25"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="66"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="67">
         <v>43646</v>
       </c>
       <c r="D21" s="12"/>
@@ -3243,25 +3280,25 @@
       <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="65"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="s">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="64" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="70" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="12"/>
@@ -3269,36 +3306,36 @@
       <c r="F23" s="25"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="79"/>
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="66"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="65"/>
       <c r="B25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="78" t="s">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="64" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="67">
         <v>43650</v>
       </c>
       <c r="D26" s="12"/>
@@ -3306,34 +3343,34 @@
       <c r="F26" s="25"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="79"/>
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="66"/>
       <c r="B27" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="83"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="25"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="79"/>
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="66"/>
       <c r="B28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="66"/>
       <c r="B29" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="81">
+      <c r="C29" s="67">
         <v>43651</v>
       </c>
       <c r="D29" s="12"/>
@@ -3341,23 +3378,23 @@
       <c r="F29" s="25"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="65"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="25"/>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A31" s="11"/>
       <c r="B31" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -3365,6 +3402,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A15"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A25"/>
@@ -3379,12 +3422,6 @@
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -3392,25 +3429,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.75" customWidth="1"/>
-    <col min="2" max="2" width="30.625" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.125" customWidth="1"/>
-    <col min="5" max="5" width="13.25" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
     <col min="7" max="7" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -3421,7 +3458,7 @@
       <c r="F1" s="46"/>
       <c r="G1" s="47"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3444,7 +3481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>8</v>
       </c>
@@ -3455,7 +3492,7 @@
       <c r="F3" s="49"/>
       <c r="G3" s="50"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -3465,7 +3502,7 @@
       <c r="C4" s="60">
         <v>43638</v>
       </c>
-      <c r="D4" s="64">
+      <c r="D4" s="83">
         <v>43642</v>
       </c>
       <c r="E4" s="12">
@@ -3476,7 +3513,7 @@
       </c>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
@@ -3495,7 +3532,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A6" s="54" t="s">
         <v>14</v>
       </c>
@@ -3516,7 +3553,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A7" s="55"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
@@ -3535,7 +3572,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A8" s="56"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
@@ -3550,7 +3587,7 @@
       </c>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A9" s="57" t="s">
         <v>18</v>
       </c>
@@ -3569,7 +3606,7 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A10" s="58"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
@@ -3586,7 +3623,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A11" s="59"/>
       <c r="B11" s="16" t="s">
         <v>21</v>
@@ -3601,7 +3638,7 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A12" s="57" t="s">
         <v>22</v>
       </c>
@@ -3616,7 +3653,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A13" s="58"/>
       <c r="B13" s="16" t="s">
         <v>24</v>
@@ -3627,7 +3664,7 @@
       <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A14" s="58"/>
       <c r="B14" s="16" t="s">
         <v>25</v>
@@ -3638,7 +3675,7 @@
       <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A15" s="59"/>
       <c r="B15" s="16" t="s">
         <v>26</v>
@@ -3649,7 +3686,7 @@
       <c r="F15" s="25"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="51" t="s">
         <v>27</v>
       </c>
@@ -3660,7 +3697,7 @@
       <c r="F16" s="52"/>
       <c r="G16" s="53"/>
     </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A17" s="57" t="s">
         <v>28</v>
       </c>
@@ -3681,7 +3718,7 @@
       </c>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A18" s="59"/>
       <c r="B18" s="16" t="s">
         <v>30</v>
@@ -3698,7 +3735,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A19" s="57" t="s">
         <v>31</v>
       </c>
@@ -3713,7 +3750,7 @@
       <c r="F19" s="25"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A20" s="58"/>
       <c r="B20" s="16" t="s">
         <v>34</v>
@@ -3724,7 +3761,7 @@
       <c r="F20" s="25"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A21" s="58"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
@@ -3737,7 +3774,7 @@
       <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A22" s="59"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
@@ -3748,7 +3785,7 @@
       <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A23" s="57" t="s">
         <v>37</v>
       </c>
@@ -3763,7 +3800,7 @@
       <c r="F23" s="25"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A24" s="58"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
@@ -3774,7 +3811,7 @@
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A25" s="59"/>
       <c r="B25" s="16" t="s">
         <v>41</v>
@@ -3785,7 +3822,7 @@
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A26" s="57" t="s">
         <v>42</v>
       </c>
@@ -3800,7 +3837,7 @@
       <c r="F26" s="25"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A27" s="58"/>
       <c r="B27" s="16" t="s">
         <v>44</v>
@@ -3811,7 +3848,7 @@
       <c r="F27" s="25"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A28" s="58"/>
       <c r="B28" s="16" t="s">
         <v>45</v>
@@ -3822,7 +3859,7 @@
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A29" s="58"/>
       <c r="B29" s="16" t="s">
         <v>46</v>
@@ -3835,7 +3872,7 @@
       <c r="F29" s="25"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A30" s="59"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
@@ -3846,7 +3883,7 @@
       <c r="F30" s="25"/>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A31" s="11"/>
       <c r="B31" s="9" t="s">
         <v>48</v>
@@ -3864,36 +3901,36 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.75" customWidth="1"/>
-    <col min="2" max="2" width="30.625" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.125" customWidth="1"/>
-    <col min="5" max="5" width="13.25" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
     <col min="7" max="7" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
-    </row>
-    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -3916,25 +3953,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="69" t="s">
+    <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="71"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="81">
+      <c r="C4" s="67">
         <v>43638</v>
       </c>
       <c r="D4" s="11"/>
@@ -3948,14 +3985,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="82"/>
+      <c r="C5" s="68"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12">
         <v>43640</v>
@@ -3965,8 +4002,8 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="80" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -3986,12 +4023,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="76"/>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="81"/>
       <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="67">
         <v>43640</v>
       </c>
       <c r="D7" s="12"/>
@@ -4003,12 +4040,12 @@
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="82"/>
       <c r="B8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="82"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12">
         <v>43641</v>
@@ -4020,14 +4057,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="78" t="s">
+    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="64" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="81">
+      <c r="C9" s="67">
         <v>43641</v>
       </c>
       <c r="D9" s="12"/>
@@ -4041,12 +4078,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="79"/>
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="66"/>
       <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="83"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12">
         <v>43642</v>
@@ -4056,12 +4093,12 @@
       </c>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="65"/>
       <c r="B11" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12">
         <v>43642</v>
@@ -4071,14 +4108,14 @@
       </c>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="64" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="81">
+      <c r="C12" s="67">
         <v>43642</v>
       </c>
       <c r="D12" s="12"/>
@@ -4090,58 +4127,58 @@
       </c>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="66"/>
       <c r="B13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="83"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="25"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="79"/>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="66"/>
       <c r="B14" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="25"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="65"/>
       <c r="B15" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="82"/>
+      <c r="C15" s="68"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="25"/>
       <c r="G15" s="14"/>
     </row>
-    <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="72" t="s">
+    <row r="16" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="78" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="79"/>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="64" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="81">
+      <c r="C17" s="67">
         <v>43643</v>
       </c>
       <c r="D17" s="12"/>
@@ -4149,12 +4186,12 @@
       <c r="F17" s="25"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
+    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="65"/>
       <c r="B18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="82"/>
+      <c r="C18" s="68"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13">
@@ -4164,14 +4201,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="78" t="s">
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A19" s="64" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="67" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="12"/>
@@ -4179,23 +4216,23 @@
       <c r="F19" s="25"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="79"/>
+    <row r="20" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="66"/>
       <c r="B20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="82"/>
+      <c r="C20" s="68"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="25"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="79"/>
+    <row r="21" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="66"/>
       <c r="B21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="81">
+      <c r="C21" s="67">
         <v>43646</v>
       </c>
       <c r="D21" s="12"/>
@@ -4203,25 +4240,25 @@
       <c r="F21" s="25"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
+    <row r="22" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="65"/>
       <c r="B22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="82"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="25"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="78" t="s">
+    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="64" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="70" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="12"/>
@@ -4229,36 +4266,36 @@
       <c r="F23" s="25"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="79"/>
+    <row r="24" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="66"/>
       <c r="B24" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="83"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="25"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="80"/>
+    <row r="25" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="65"/>
       <c r="B25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="82"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="25"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="78" t="s">
+    <row r="26" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="64" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="81">
+      <c r="C26" s="67">
         <v>43650</v>
       </c>
       <c r="D26" s="12"/>
@@ -4266,34 +4303,34 @@
       <c r="F26" s="25"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="79"/>
+    <row r="27" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="66"/>
       <c r="B27" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="83"/>
+      <c r="C27" s="69"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="25"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="79"/>
+    <row r="28" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="66"/>
       <c r="B28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="25"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="79"/>
+    <row r="29" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="66"/>
       <c r="B29" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="81">
+      <c r="C29" s="67">
         <v>43651</v>
       </c>
       <c r="D29" s="12"/>
@@ -4301,23 +4338,23 @@
       <c r="F29" s="25"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
+    <row r="30" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="65"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="25"/>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A31" s="11"/>
       <c r="B31" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -4325,6 +4362,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A15"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A22"/>
     <mergeCell ref="A23:A25"/>
@@ -4339,12 +4382,6 @@
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="C29:C31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A15"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>